<commit_message>
Add E-Change,and adding images by Nagai is as F-change.
</commit_message>
<xml_diff>
--- a/01_document/04_ソフトウェア実装プロセス/01_ソフトウェア要件定義/01_ユーザー認証.xlsx
+++ b/01_document/04_ソフトウェア実装プロセス/01_ソフトウェア要件定義/01_ユーザー認証.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18229"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\13.Git\TeamCafeAuLait\01_document\04_ソフトウェア実装プロセス\01_ソフトウェア要件定義\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shoji\Documents\TeamCafeAuLait\01_document\04_ソフトウェア実装プロセス\01_ソフトウェア要件定義\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
     <sheet name="Message" sheetId="4" r:id="rId5"/>
     <sheet name="改訂履歴" sheetId="5" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="174">
   <si>
     <t>ユーザー認証</t>
     <rPh sb="4" eb="6">
@@ -676,13 +676,6 @@
   </si>
   <si>
     <t>No.</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>　　→パスワードとIDテキストボックスの背景色を赤にし、エラーメッセージを表示する、そして入力された内容をリセットする。メッセージは[Message]シートA-4に記載する。[A-4](改訂A-1)</t>
-    <rPh sb="93" eb="95">
-      <t>カイテイ</t>
-    </rPh>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -1635,10 +1628,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>改訂D</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>[カード認証]
 ④カードのデータ取得に成功した場合
 →メッセージを表示し、メッセージ内のOKボタンが押下された時、共通画面に遷移する。
@@ -1691,11 +1680,80 @@
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
+  <si>
+    <t>第四回レビュー指摘対応</t>
+    <rPh sb="0" eb="1">
+      <t>ダイ</t>
+    </rPh>
+    <rPh sb="1" eb="2">
+      <t>ヨン</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>カイ</t>
+    </rPh>
+    <rPh sb="7" eb="9">
+      <t>シテキ</t>
+    </rPh>
+    <rPh sb="9" eb="11">
+      <t>タイオウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>改訂E</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>第五回レビュー指摘対応</t>
+    <rPh sb="0" eb="1">
+      <t>ダイ</t>
+    </rPh>
+    <rPh sb="1" eb="2">
+      <t>ゴ</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>カイ</t>
+    </rPh>
+    <rPh sb="7" eb="9">
+      <t>シテキ</t>
+    </rPh>
+    <rPh sb="9" eb="11">
+      <t>タイオウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">[認証画面]
+「パスワードとIDテキストボックスの背景色を赤にし、エラーメッセージを表示する、そして入力された内容をリセットする。」
+</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>[認証画面]
+「パスワードとIDテキストボックスの背景色を赤にし、エラーメッセージを表示するが、入力されたIDとパスワードはそのままにする。」</t>
+    <rPh sb="1" eb="3">
+      <t>ニンショウ</t>
+    </rPh>
+    <rPh sb="3" eb="5">
+      <t>ガメン</t>
+    </rPh>
+    <rPh sb="48" eb="50">
+      <t>ニュウリョク</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>　　→パスワードとIDテキストボックスの背景色を赤にし、エラーメッセージを表示するが、入力されたIDとパスワードはそのままにする。メッセージは[Message]シートA-4に記載する。[A-4](改訂A-1)(改訂E-1)</t>
+    <rPh sb="98" eb="100">
+      <t>カイテイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1994,7 +2052,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="図 1"/>
+        <xdr:cNvPr id="2" name="図 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -2032,7 +2096,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="図 2"/>
+        <xdr:cNvPr id="3" name="図 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -2075,7 +2145,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="図 2"/>
+        <xdr:cNvPr id="3" name="図 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -2118,7 +2194,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="図 2"/>
+        <xdr:cNvPr id="3" name="図 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -2409,30 +2491,32 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A6"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="9" style="2" customWidth="1"/>
     <col min="2" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
@@ -2448,36 +2532,38 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G44"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
+    <sheetView showGridLines="0" topLeftCell="A5" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F20" sqref="F19:F20"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="9" style="2" customWidth="1"/>
     <col min="2" max="2" width="9" style="2"/>
-    <col min="3" max="3" width="31.7265625" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="45.26953125" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="41.26953125" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.7265625" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="23.26953125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.75" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="45.25" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="41.25" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.75" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.25" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
@@ -2494,7 +2580,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.15">
       <c r="B7" s="3">
         <v>1</v>
       </c>
@@ -2508,7 +2594,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
       <c r="B8" s="3">
         <f t="shared" ref="B8:B13" si="0">ROW()-6</f>
         <v>2</v>
@@ -2523,7 +2609,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.15">
       <c r="B9" s="3">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -2538,7 +2624,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.15">
       <c r="B10" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -2553,7 +2639,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.15">
       <c r="B11" s="3">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -2568,7 +2654,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.15">
       <c r="B12" s="3">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -2583,25 +2669,25 @@
         <v>63</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.15">
       <c r="B13" s="23">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="C13" s="23" t="s">
+        <v>120</v>
+      </c>
+      <c r="D13" s="23" t="s">
         <v>121</v>
       </c>
-      <c r="D13" s="23" t="s">
+      <c r="E13" s="23" t="s">
+        <v>123</v>
+      </c>
+      <c r="F13" s="32" t="s">
         <v>122</v>
       </c>
-      <c r="E13" s="23" t="s">
-        <v>124</v>
-      </c>
-      <c r="F13" s="32" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A15" s="2" t="s">
         <v>65</v>
       </c>
@@ -2612,7 +2698,7 @@
       <c r="F15" s="4"/>
       <c r="G15" s="5"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.15">
       <c r="B16" s="4"/>
       <c r="C16" s="4"/>
       <c r="D16" s="4"/>
@@ -2620,12 +2706,12 @@
       <c r="F16" s="4"/>
       <c r="G16" s="5"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.15">
       <c r="B17" s="2" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A19" s="2" t="s">
         <v>66</v>
       </c>
@@ -2636,7 +2722,7 @@
       <c r="F19" s="4"/>
       <c r="G19" s="5"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.15">
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
       <c r="D20" s="4"/>
@@ -2644,7 +2730,7 @@
       <c r="F20" s="4"/>
       <c r="G20" s="5"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.15">
       <c r="B21" s="2" t="s">
         <v>58</v>
       </c>
@@ -2654,24 +2740,24 @@
       <c r="F21" s="6"/>
       <c r="G21" s="6"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.15">
       <c r="B22" s="19" t="s">
-        <v>80</v>
+        <v>173</v>
       </c>
       <c r="C22" s="20"/>
       <c r="D22" s="20"/>
       <c r="E22" s="20"/>
       <c r="F22" s="20"/>
-      <c r="G22" s="6"/>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G22" s="20"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.15">
       <c r="C23" s="6"/>
       <c r="D23" s="6"/>
       <c r="E23" s="6"/>
       <c r="F23" s="6"/>
       <c r="G23" s="6"/>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.15">
       <c r="B24" s="2" t="s">
         <v>59</v>
       </c>
@@ -2681,7 +2767,7 @@
       <c r="F24" s="6"/>
       <c r="G24" s="6"/>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.15">
       <c r="B25" s="2" t="s">
         <v>61</v>
       </c>
@@ -2691,14 +2777,14 @@
       <c r="F25" s="6"/>
       <c r="G25" s="6"/>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.15">
       <c r="C26" s="6"/>
       <c r="D26" s="6"/>
       <c r="E26" s="6"/>
       <c r="F26" s="6"/>
       <c r="G26" s="6"/>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A27" s="2" t="s">
         <v>67</v>
       </c>
@@ -2708,14 +2794,14 @@
       <c r="F27" s="6"/>
       <c r="G27" s="6"/>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.15">
       <c r="C28" s="6"/>
       <c r="D28" s="6"/>
       <c r="E28" s="6"/>
       <c r="F28" s="6"/>
       <c r="G28" s="6"/>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.15">
       <c r="B29" s="2" t="s">
         <v>24</v>
       </c>
@@ -2725,14 +2811,14 @@
       <c r="F29" s="6"/>
       <c r="G29" s="6"/>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.15">
       <c r="C30" s="6"/>
       <c r="D30" s="6"/>
       <c r="E30" s="6"/>
       <c r="F30" s="6"/>
       <c r="G30" s="6"/>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.15">
       <c r="C31" s="7"/>
       <c r="D31" s="3" t="s">
         <v>25</v>
@@ -2747,7 +2833,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.15">
       <c r="C32" s="7" t="s">
         <v>29</v>
       </c>
@@ -2764,7 +2850,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.15">
       <c r="C33" s="7" t="s">
         <v>33</v>
       </c>
@@ -2781,9 +2867,9 @@
         <v>60</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A35" s="19" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B35" s="19"/>
       <c r="C35" s="20"/>
@@ -2792,16 +2878,16 @@
       <c r="F35" s="6"/>
       <c r="G35" s="6"/>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A36" s="19"/>
       <c r="B36" s="19"/>
       <c r="C36" s="19"/>
       <c r="D36" s="19"/>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A37" s="19"/>
       <c r="B37" s="19" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C37" s="20"/>
       <c r="D37" s="20"/>
@@ -2809,10 +2895,10 @@
       <c r="F37" s="6"/>
       <c r="G37" s="6"/>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A38" s="19"/>
       <c r="B38" s="19" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C38" s="20"/>
       <c r="D38" s="20"/>
@@ -2820,25 +2906,25 @@
       <c r="F38" s="6"/>
       <c r="G38" s="6"/>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.15">
       <c r="B40" s="19" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C40" s="19"/>
       <c r="D40" s="19"/>
       <c r="E40" s="19"/>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.15">
       <c r="B41" s="19" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C41" s="19"/>
       <c r="D41" s="19"/>
       <c r="E41" s="19"/>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A43" s="19" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B43" s="19"/>
       <c r="C43" s="20"/>
@@ -2847,9 +2933,9 @@
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.15">
       <c r="B44" s="19" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C44" s="19"/>
     </row>
@@ -2865,41 +2951,41 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J15"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A12" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
       <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="9" style="19" customWidth="1"/>
     <col min="2" max="2" width="9" style="19"/>
-    <col min="3" max="3" width="16.26953125" style="19" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.7265625" style="19" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.90625" style="19" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.25" style="19" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.75" style="19" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.875" style="19" bestFit="1" customWidth="1"/>
     <col min="6" max="16384" width="9" style="19"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A1" s="25" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A3" s="25" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A4" s="19" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="B6" s="19" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B6" s="19" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A8" s="19" t="s">
         <v>5</v>
       </c>
@@ -2916,7 +3002,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.15">
       <c r="B9" s="23">
         <v>1</v>
       </c>
@@ -2930,7 +3016,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.15">
       <c r="B10" s="23">
         <v>2</v>
       </c>
@@ -2941,17 +3027,17 @@
         <v>77</v>
       </c>
       <c r="E10" s="23" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="B12" s="19" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B12" s="19" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.15">
       <c r="B14" s="31" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C14" s="31"/>
       <c r="D14" s="31"/>
@@ -2962,9 +3048,9 @@
       <c r="I14" s="31"/>
       <c r="J14" s="31"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.15">
       <c r="B15" s="31" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C15" s="31"/>
       <c r="D15" s="31"/>
@@ -2988,40 +3074,40 @@
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="55" zoomScaleNormal="55" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="2" width="9" style="19"/>
-    <col min="3" max="3" width="21.26953125" style="19" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.7265625" style="19" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.25" style="19" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.75" style="19" bestFit="1" customWidth="1"/>
     <col min="5" max="16384" width="9" style="19"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A1" s="25" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A3" s="25" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="25" t="s">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A4" s="19" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="19" t="s">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A6" s="25" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="25" t="s">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A7" s="19" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="19" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A9" s="19" t="s">
         <v>5</v>
       </c>
@@ -3038,88 +3124,88 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B10" s="23">
         <v>1</v>
       </c>
       <c r="C10" s="23" t="s">
+        <v>131</v>
+      </c>
+      <c r="D10" s="23" t="s">
         <v>132</v>
       </c>
-      <c r="D10" s="23" t="s">
+      <c r="E10" s="23" t="s">
         <v>133</v>
       </c>
-      <c r="E10" s="23" t="s">
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="B12" s="19" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="B14" s="19" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B12" s="19" t="s">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="B16" s="19" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B14" s="19" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B16" s="19" t="s">
+    <row r="17" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B17" s="19" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B17" s="19" t="s">
+    <row r="18" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B18" s="19" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B19" s="19" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="21" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B21" s="19" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="22" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B22" s="19" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="23" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B23" s="19" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="25" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B25" s="19" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B18" s="19" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B19" s="19" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B21" s="19" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B22" s="19" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B23" s="19" t="s">
+    <row r="26" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B26" s="19" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="28" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B28" s="19" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="25" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B25" s="19" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="26" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B26" s="19" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="28" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B28" s="19" t="s">
+    <row r="29" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B29" s="19" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="30" spans="2:2" x14ac:dyDescent="0.15">
+      <c r="B30" s="19" t="s">
         <v>145</v>
-      </c>
-    </row>
-    <row r="29" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B29" s="19" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="30" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B30" s="19" t="s">
-        <v>146</v>
       </c>
     </row>
   </sheetData>
@@ -3135,27 +3221,27 @@
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="9" style="2" customWidth="1"/>
-    <col min="2" max="2" width="49.36328125" style="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.08984375" style="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.6328125" style="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="46.08984375" style="2" customWidth="1"/>
-    <col min="6" max="6" width="23.90625" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.90625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="49.375" style="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.125" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.625" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="46.125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="23.875" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.875" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.15">
       <c r="B2" s="13"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.15">
       <c r="B3" s="3" t="s">
         <v>40</v>
       </c>
@@ -3172,10 +3258,10 @@
         <v>43</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="52" x14ac:dyDescent="0.2">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="54" x14ac:dyDescent="0.15">
       <c r="B4" s="3" t="s">
         <v>52</v>
       </c>
@@ -3195,7 +3281,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="52" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" ht="54" x14ac:dyDescent="0.15">
       <c r="B5" s="3" t="s">
         <v>47</v>
       </c>
@@ -3215,7 +3301,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="52" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" ht="54" x14ac:dyDescent="0.15">
       <c r="B6" s="3" t="s">
         <v>50</v>
       </c>
@@ -3235,9 +3321,9 @@
         <v>55</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="52" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" ht="54" x14ac:dyDescent="0.15">
       <c r="B7" s="23" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C7" s="23" t="s">
         <v>44</v>
@@ -3246,44 +3332,44 @@
         <v>45</v>
       </c>
       <c r="E7" s="26" t="s">
+        <v>99</v>
+      </c>
+      <c r="F7" s="26" t="s">
+        <v>96</v>
+      </c>
+      <c r="G7" s="28" t="s">
+        <v>95</v>
+      </c>
+      <c r="H7" s="19" t="s">
         <v>100</v>
       </c>
-      <c r="F7" s="26" t="s">
-        <v>97</v>
-      </c>
-      <c r="G7" s="28" t="s">
-        <v>96</v>
-      </c>
-      <c r="H7" s="19" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="52" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:8" ht="40.5" x14ac:dyDescent="0.15">
       <c r="B8" s="23" t="s">
+        <v>87</v>
+      </c>
+      <c r="C8" s="23" t="s">
         <v>88</v>
-      </c>
-      <c r="C8" s="23" t="s">
-        <v>89</v>
       </c>
       <c r="D8" s="23" t="s">
         <v>45</v>
       </c>
       <c r="E8" s="26" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F8" s="27" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G8" s="28" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H8" s="19" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="52" x14ac:dyDescent="0.2">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="54" x14ac:dyDescent="0.15">
       <c r="B9" s="23" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C9" s="23" t="s">
         <v>48</v>
@@ -3292,21 +3378,21 @@
         <v>46</v>
       </c>
       <c r="E9" s="26" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F9" s="27" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="G9" s="28" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="H9" s="19" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="39" x14ac:dyDescent="0.2">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="40.5" x14ac:dyDescent="0.15">
       <c r="B10" s="23" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C10" s="23" t="s">
         <v>48</v>
@@ -3315,39 +3401,39 @@
         <v>45</v>
       </c>
       <c r="E10" s="26" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="F10" s="27" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="G10" s="28" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="H10" s="19" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="65" x14ac:dyDescent="0.2">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="67.5" x14ac:dyDescent="0.15">
       <c r="B11" s="23" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C11" s="23" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D11" s="23" t="s">
         <v>45</v>
       </c>
       <c r="E11" s="26" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F11" s="27" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="G11" s="28" t="s">
+        <v>150</v>
+      </c>
+      <c r="H11" s="19" t="s">
         <v>151</v>
-      </c>
-      <c r="H11" s="19" t="s">
-        <v>152</v>
       </c>
     </row>
   </sheetData>
@@ -3358,20 +3444,22 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:G12"/>
+  <dimension ref="B2:G13"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="9" customWidth="1"/>
-    <col min="4" max="4" width="22.36328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.453125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.90625" customWidth="1"/>
-    <col min="7" max="7" width="27.6328125" customWidth="1"/>
+    <col min="4" max="4" width="22.375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.875" customWidth="1"/>
+    <col min="7" max="7" width="27.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:7" x14ac:dyDescent="0.15">
       <c r="B2" s="15" t="s">
         <v>78</v>
       </c>
@@ -3389,7 +3477,7 @@
       </c>
       <c r="G2" s="34"/>
     </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:7" x14ac:dyDescent="0.15">
       <c r="B3" s="16"/>
       <c r="C3" s="16"/>
       <c r="D3" s="16"/>
@@ -3401,9 +3489,9 @@
         <v>72</v>
       </c>
     </row>
-    <row r="4" spans="2:7" ht="156" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:7" ht="162" x14ac:dyDescent="0.15">
       <c r="B4" s="30" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C4" s="14">
         <v>1</v>
@@ -3415,13 +3503,13 @@
         <v>42859</v>
       </c>
       <c r="F4" s="22" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G4" s="22" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="5" spans="2:7" ht="104" x14ac:dyDescent="0.2">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" ht="108" x14ac:dyDescent="0.15">
       <c r="B5" s="29"/>
       <c r="C5" s="16">
         <v>2</v>
@@ -3433,13 +3521,13 @@
         <v>42859</v>
       </c>
       <c r="F5" s="21" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G5" s="22" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="6" spans="2:7" ht="91" x14ac:dyDescent="0.2">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" ht="94.5" x14ac:dyDescent="0.15">
       <c r="B6" s="29"/>
       <c r="C6" s="16">
         <v>3</v>
@@ -3451,128 +3539,146 @@
         <v>42859</v>
       </c>
       <c r="F6" s="21" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G6" s="22" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="7" spans="2:7" ht="104" x14ac:dyDescent="0.2">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" ht="108" x14ac:dyDescent="0.15">
       <c r="B7" s="14" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C7" s="16">
         <v>1</v>
       </c>
       <c r="D7" s="14" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E7" s="24">
         <v>42861</v>
       </c>
       <c r="F7" s="21" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G7" s="22" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="8" spans="2:7" ht="91" x14ac:dyDescent="0.2">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" ht="94.5" x14ac:dyDescent="0.15">
       <c r="B8" s="15" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C8" s="16">
         <v>1</v>
       </c>
       <c r="D8" s="14" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E8" s="24">
         <v>42875</v>
       </c>
       <c r="F8" s="21" t="s">
+        <v>113</v>
+      </c>
+      <c r="G8" s="22" t="s">
         <v>114</v>
       </c>
-      <c r="G8" s="22" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="9" spans="2:7" ht="91" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="2:7" ht="94.5" x14ac:dyDescent="0.15">
       <c r="B9" s="29" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C9" s="16">
         <v>2</v>
       </c>
       <c r="D9" s="14" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E9" s="24">
         <v>42875</v>
       </c>
       <c r="F9" s="21" t="s">
+        <v>118</v>
+      </c>
+      <c r="G9" s="22" t="s">
         <v>119</v>
       </c>
-      <c r="G9" s="22" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="10" spans="2:7" ht="91" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="2:7" ht="94.5" x14ac:dyDescent="0.15">
       <c r="B10" s="16" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C10" s="16">
         <v>3</v>
       </c>
       <c r="D10" s="14" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E10" s="24">
         <v>42875</v>
       </c>
       <c r="F10" s="21" t="s">
+        <v>146</v>
+      </c>
+      <c r="G10" s="22" t="s">
         <v>147</v>
       </c>
-      <c r="G10" s="22" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="11" spans="2:7" ht="143" x14ac:dyDescent="0.2">
-      <c r="B11" s="14" t="s">
-        <v>164</v>
+    </row>
+    <row r="11" spans="2:7" ht="135" x14ac:dyDescent="0.15">
+      <c r="B11" s="15" t="s">
+        <v>163</v>
       </c>
       <c r="C11" s="16">
         <v>1</v>
       </c>
       <c r="D11" s="14" t="s">
-        <v>106</v>
+        <v>168</v>
       </c>
       <c r="E11" s="24">
         <v>42903</v>
       </c>
       <c r="F11" s="21" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="G11" s="22" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="12" spans="2:7" ht="52" x14ac:dyDescent="0.2">
-      <c r="B12" s="14" t="s">
-        <v>165</v>
-      </c>
+        <v>167</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" ht="54" x14ac:dyDescent="0.15">
+      <c r="B12" s="16"/>
       <c r="C12" s="16">
         <v>2</v>
       </c>
       <c r="D12" s="14" t="s">
-        <v>106</v>
+        <v>168</v>
       </c>
       <c r="E12" s="24">
         <v>42903</v>
       </c>
       <c r="F12" s="21"/>
       <c r="G12" s="22" t="s">
-        <v>168</v>
+        <v>166</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7" ht="94.5" x14ac:dyDescent="0.15">
+      <c r="B13" s="14" t="s">
+        <v>169</v>
+      </c>
+      <c r="C13" s="16">
+        <v>1</v>
+      </c>
+      <c r="D13" s="14" t="s">
+        <v>170</v>
+      </c>
+      <c r="E13" s="24">
+        <v>42925</v>
+      </c>
+      <c r="F13" s="22" t="s">
+        <v>171</v>
+      </c>
+      <c r="G13" s="22" t="s">
+        <v>172</v>
       </c>
     </row>
   </sheetData>

</xml_diff>